<commit_message>
save tests into folder
</commit_message>
<xml_diff>
--- a/base.xlsx
+++ b/base.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Hoja 1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>PARAMETERS</t>
   </si>
@@ -19,37 +19,49 @@
     <t>RESULT</t>
   </si>
   <si>
-    <t>CARD BRAND</t>
-  </si>
-  <si>
-    <t>EMAIL</t>
-  </si>
-  <si>
-    <t>PHONE</t>
-  </si>
-  <si>
-    <t>PR_ID</t>
-  </si>
-  <si>
-    <t>PAYMENT FLOW</t>
-  </si>
-  <si>
-    <t>AMOUNT</t>
-  </si>
-  <si>
-    <t>PR_TYPE</t>
-  </si>
-  <si>
-    <t>STATUS_TEST</t>
-  </si>
-  <si>
-    <t>(IF REQUEST GOES BAD PRINT HERE</t>
-  </si>
-  <si>
-    <t>Guest</t>
-  </si>
-  <si>
-    <t>HOSTED_CHECKOUT</t>
+    <t>Case ID</t>
+  </si>
+  <si>
+    <t>Card Brand</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>PR ID</t>
+  </si>
+  <si>
+    <t>Payment Flow</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>PR Type</t>
+  </si>
+  <si>
+    <t>Status Test</t>
+  </si>
+  <si>
+    <t>Visa</t>
+  </si>
+  <si>
+    <t>G@gmail.com</t>
+  </si>
+  <si>
+    <t>9131e884-faf2-4416-ad26-4e29a8a8a0fd</t>
+  </si>
+  <si>
+    <t>GUEST</t>
+  </si>
+  <si>
+    <t>HXO</t>
+  </si>
+  <si>
+    <t>Ok</t>
   </si>
 </sst>
 </file>
@@ -69,7 +81,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -78,20 +90,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF9900"/>
-        <bgColor rgb="FFFF9900"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF93C47D"/>
-        <bgColor rgb="FF93C47D"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF3F3F3"/>
-        <bgColor rgb="FFF3F3F3"/>
+        <fgColor rgb="FF6AA84F"/>
+        <bgColor rgb="FF6AA84F"/>
       </patternFill>
     </fill>
   </fills>
@@ -101,7 +101,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -109,15 +109,7 @@
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -336,12 +328,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="15.5"/>
-    <col customWidth="1" min="2" max="2" width="16.5"/>
-    <col customWidth="1" min="5" max="5" width="15.38"/>
-    <col customWidth="1" min="6" max="6" width="19.0"/>
-    <col customWidth="1" min="7" max="7" width="20.25"/>
-    <col customWidth="1" min="10" max="10" width="32.63"/>
+    <col customWidth="1" min="8" max="8" width="18.38"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -352,68 +339,70 @@
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="4"/>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="H2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="K2" s="3"/>
     </row>
-    <row r="3" ht="19.5" customHeight="1">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="7" t="s">
+    <row r="3">
+      <c r="A3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="7" t="s">
+      <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
+      <c r="D3" s="3">
+        <v>1.14324243E8</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E3">
-      <formula1>"Guest,Register"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G3">
-      <formula1>"HOSTED_CHECKOUT,LINK_PAGO,SUBSCRIPCION"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="A3:C3">
-      <formula1>"RANDOM,CUSTOM"</formula1>
-    </dataValidation>
-  </dataValidations>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
environments dev stage, format card, fill email normalized, finally for cluster before for initialization
</commit_message>
<xml_diff>
--- a/base.xlsx
+++ b/base.xlsx
@@ -25,7 +25,7 @@
     <t>Case ID</t>
   </si>
   <si>
-    <t>Card Brand</t>
+    <t>Card Number</t>
   </si>
   <si>
     <t>Email</t>
@@ -57,7 +57,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -69,6 +69,18 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -119,7 +131,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -127,29 +139,35 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -459,20 +477,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="8" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="8" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="9" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="10" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="9" width="18.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="9" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="9" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="9" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="9" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="10" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="10" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="9" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="10" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="10" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="11" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="10" width="18.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="12" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="10" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="10" width="13.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2" t="s">
@@ -483,44 +501,44 @@
       <c r="F1" s="3"/>
       <c r="G1" s="4"/>
       <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="5" t="s">
+      <c r="I1" s="5"/>
+      <c r="J1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="K1" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
-      <c r="A2" s="6" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="5"/>
+      <c r="K2" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>